<commit_message>
Updated analysis to include fibon data
</commit_message>
<xml_diff>
--- a/ANALYSIS/fibon.xlsx
+++ b/ANALYSIS/fibon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="4200" windowWidth="18400" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="2040" yWindow="1100" windowWidth="14880" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>n</t>
   </si>
@@ -100,14 +100,32 @@
   </si>
   <si>
     <t>Xsact-Ref-Peak</t>
+  </si>
+  <si>
+    <t>MAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEOMEAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="7">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -139,11 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +494,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1041,6 +1061,114 @@
         <v>1.1651376189506399E-4</v>
       </c>
     </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1">
+        <f>MAX(B2:B19)</f>
+        <v>0.37272163533592501</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" ref="C21:I21" si="0">MAX(C2:C19)</f>
+        <v>0.50299942897798899</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4402295259922203E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.58364813663113402</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5419426558113604E-2</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>153.52078610223401</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>540.33160571694305</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6235951545889807E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1">
+        <f>MEDIAN(B2:B19)</f>
+        <v>0.26798363272336601</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" ref="C22:I22" si="1">MEDIAN(C2:C19)</f>
+        <v>-1.9332663423260949E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9623213981109E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.465304567087565E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>2.46445602871346E-2</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="1"/>
+        <v>29.500523858660898</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="1"/>
+        <v>12.780651374538401</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2193878617251251E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1">
+        <f>GEOMEAN(B2:B19)</f>
+        <v>0.27214061209762902</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <f t="shared" ref="C23:I23" si="2">GEOMEAN(D2:D19)</f>
+        <v>1.6172227565266553E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2407410308621919E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4544263338556783E-2</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="2"/>
+        <v>31.143617535132961</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="2"/>
+        <v>10.223301308017163</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="2"/>
+        <v>7.8318303717880291E-4</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">

</xml_diff>